<commit_message>
correzione versione test 369
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111KIRANETXXXX/KIRANET/FIDCARE/5.25/accreditamento-checklist_V8.2.2.xlsx
+++ b/GATEWAY/A1#111KIRANETXXXX/KIRANET/FIDCARE/5.25/accreditamento-checklist_V8.2.2.xlsx
@@ -824,13 +824,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 0" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-02-04 09:44:03Z</t>
-  </si>
-  <si>
-    <t>81f37aeff8be548f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.869380fef70f904daebe414a78aa4e9979b470b88449625255662442c6b36217.a3758cf2e9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-02-04 17:36:35Z</t>
+  </si>
+  <si>
+    <t>a40373f002aa7431</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.869380fef70f904daebe414a78aa4e9979b470b88449625255662442c6b36217.71f90076fe^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT0</t>

</xml_diff>